<commit_message>
added search and suggestion of medicin name
</commit_message>
<xml_diff>
--- a/sales.xlsx
+++ b/sales.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>customer_name</t>
   </si>
@@ -31,7 +31,19 @@
     <t>siddharth</t>
   </si>
   <si>
+    <t>nitesh</t>
+  </si>
+  <si>
+    <t>siddhu</t>
+  </si>
+  <si>
     <t>vada pav</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -389,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,13 +426,27 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>